<commit_message>
Compcopy and order management record saving
</commit_message>
<xml_diff>
--- a/SkillMatrix.Web/wwwroot/Files/Templates/Template_QualityChecks.xlsx
+++ b/SkillMatrix.Web/wwwroot/Files/Templates/Template_QualityChecks.xlsx
@@ -12,7 +12,7 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$2:$Z$6</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$Z$5</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
 </workbook>
@@ -683,10 +683,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A2:Z6"/>
+  <dimension ref="A1:Z5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="91" workbookViewId="0">
-      <selection activeCell="Y7" sqref="Y7"/>
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -716,131 +716,211 @@
     <col min="26" max="26" width="10.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:26" ht="37.5" customHeight="1">
-      <c r="A2" s="3" t="s">
+    <row r="1" spans="1:26" ht="37.5" customHeight="1">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="F1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="G1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="H1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="I2" s="4" t="s">
+      <c r="I1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="J2" s="6" t="s">
+      <c r="J1" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="K2" s="6" t="s">
+      <c r="K1" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="L2" s="6" t="s">
+      <c r="L1" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="M2" s="6" t="s">
+      <c r="M1" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="N2" s="7" t="s">
+      <c r="N1" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="O2" s="8" t="s">
+      <c r="O1" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="P2" s="3" t="s">
+      <c r="P1" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="Q2" s="4" t="s">
+      <c r="Q1" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="R2" s="9" t="s">
+      <c r="R1" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="S2" s="9" t="s">
+      <c r="S1" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="T2" s="9" t="s">
+      <c r="T1" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="U2" s="9" t="s">
+      <c r="U1" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="V2" s="9" t="s">
+      <c r="V1" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="W2" s="10" t="s">
+      <c r="W1" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="X2" s="9" t="s">
+      <c r="X1" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="Y2" s="9" t="s">
+      <c r="Y1" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="Z2" s="2" t="s">
+      <c r="Z1" s="2" t="s">
         <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:26">
+      <c r="A2" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" s="13">
+        <v>44378</v>
+      </c>
+      <c r="D2" s="13">
+        <v>44384</v>
+      </c>
+      <c r="E2" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="F2" s="14">
+        <v>5670654</v>
+      </c>
+      <c r="G2" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="H2" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="I2" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="J2" s="14">
+        <v>25</v>
+      </c>
+      <c r="K2" s="14">
+        <v>30</v>
+      </c>
+      <c r="L2" s="14">
+        <v>30</v>
+      </c>
+      <c r="M2" s="14">
+        <v>15</v>
+      </c>
+      <c r="N2" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="O2" s="16">
+        <v>100</v>
+      </c>
+      <c r="P2" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q2" s="25" t="s">
+        <v>21</v>
+      </c>
+      <c r="R2" s="16" t="s">
+        <v>47</v>
+      </c>
+      <c r="S2" s="16">
+        <v>25</v>
+      </c>
+      <c r="T2" s="16">
+        <v>30</v>
+      </c>
+      <c r="U2" s="16">
+        <v>30</v>
+      </c>
+      <c r="V2" s="16">
+        <v>15</v>
+      </c>
+      <c r="W2" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="X2" s="1">
+        <v>100</v>
+      </c>
+      <c r="Y2" s="16">
+        <v>0</v>
+      </c>
+      <c r="Z2" s="16" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:26">
-      <c r="A3" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="B3" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="C3" s="13">
+      <c r="A3" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="B3" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="C3" s="20">
         <v>44378</v>
       </c>
-      <c r="D3" s="13">
+      <c r="D3" s="20">
         <v>44384</v>
       </c>
-      <c r="E3" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="F3" s="14">
-        <v>5670654</v>
-      </c>
-      <c r="G3" s="14" t="s">
-        <v>44</v>
-      </c>
-      <c r="H3" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="I3" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="J3" s="14">
-        <v>25</v>
-      </c>
-      <c r="K3" s="14">
+      <c r="E3" s="21" t="s">
+        <v>31</v>
+      </c>
+      <c r="F3" s="21">
+        <v>5669257</v>
+      </c>
+      <c r="G3" s="21" t="s">
+        <v>23</v>
+      </c>
+      <c r="H3" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="I3" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="J3" s="21">
+        <v>25</v>
+      </c>
+      <c r="K3" s="21">
+        <v>25</v>
+      </c>
+      <c r="L3" s="21">
         <v>30</v>
       </c>
-      <c r="L3" s="14">
-        <v>30</v>
-      </c>
-      <c r="M3" s="14">
+      <c r="M3" s="21">
         <v>15</v>
       </c>
-      <c r="N3" s="15" t="s">
+      <c r="N3" s="22" t="s">
         <v>26</v>
       </c>
       <c r="O3" s="16">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="P3" s="11" t="s">
         <v>20</v>
@@ -848,79 +928,65 @@
       <c r="Q3" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="R3" s="16" t="s">
-        <v>47</v>
-      </c>
-      <c r="S3" s="16">
-        <v>25</v>
-      </c>
-      <c r="T3" s="16">
-        <v>30</v>
-      </c>
-      <c r="U3" s="16">
-        <v>30</v>
-      </c>
-      <c r="V3" s="16">
-        <v>15</v>
-      </c>
-      <c r="W3" s="17" t="s">
-        <v>27</v>
-      </c>
-      <c r="X3" s="1">
-        <v>100</v>
-      </c>
-      <c r="Y3" s="16">
-        <v>0</v>
-      </c>
-      <c r="Z3" s="16" t="s">
-        <v>28</v>
-      </c>
+      <c r="R3" s="23"/>
+      <c r="S3" s="23"/>
+      <c r="T3" s="23"/>
+      <c r="U3" s="23"/>
+      <c r="V3" s="23"/>
+      <c r="W3" s="24"/>
+      <c r="X3" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Y3" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="Z3" s="23"/>
     </row>
     <row r="4" spans="1:26">
-      <c r="A4" s="18" t="s">
-        <v>29</v>
-      </c>
-      <c r="B4" s="19" t="s">
+      <c r="A4" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="B4" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="C4" s="13">
+        <v>44378</v>
+      </c>
+      <c r="D4" s="13">
+        <v>44384</v>
+      </c>
+      <c r="E4" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="F4" s="14">
+        <v>5668818</v>
+      </c>
+      <c r="G4" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="H4" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="I4" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="J4" s="14">
+        <v>25</v>
+      </c>
+      <c r="K4" s="14">
         <v>30</v>
       </c>
-      <c r="C4" s="20">
-        <v>44378</v>
-      </c>
-      <c r="D4" s="20">
-        <v>44384</v>
-      </c>
-      <c r="E4" s="21" t="s">
-        <v>31</v>
-      </c>
-      <c r="F4" s="21">
-        <v>5669257</v>
-      </c>
-      <c r="G4" s="21" t="s">
-        <v>23</v>
-      </c>
-      <c r="H4" s="21" t="s">
-        <v>32</v>
-      </c>
-      <c r="I4" s="21" t="s">
-        <v>25</v>
-      </c>
-      <c r="J4" s="21">
-        <v>25</v>
-      </c>
-      <c r="K4" s="21">
-        <v>25</v>
-      </c>
-      <c r="L4" s="21">
+      <c r="L4" s="14">
         <v>30</v>
       </c>
-      <c r="M4" s="21">
+      <c r="M4" s="14">
         <v>15</v>
       </c>
-      <c r="N4" s="22" t="s">
-        <v>26</v>
+      <c r="N4" s="14" t="s">
+        <v>50</v>
       </c>
       <c r="O4" s="16">
-        <v>95</v>
+        <v>100</v>
       </c>
       <c r="P4" s="11" t="s">
         <v>20</v>
@@ -928,26 +994,40 @@
       <c r="Q4" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="R4" s="23"/>
-      <c r="S4" s="23"/>
-      <c r="T4" s="23"/>
-      <c r="U4" s="23"/>
-      <c r="V4" s="23"/>
-      <c r="W4" s="24"/>
-      <c r="X4" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="Y4" s="16" t="s">
-        <v>33</v>
-      </c>
-      <c r="Z4" s="23"/>
+      <c r="R4" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="S4" s="16">
+        <v>25</v>
+      </c>
+      <c r="T4" s="16">
+        <v>25</v>
+      </c>
+      <c r="U4" s="16">
+        <v>30</v>
+      </c>
+      <c r="V4" s="16">
+        <v>15</v>
+      </c>
+      <c r="W4" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="X4" s="1">
+        <v>95</v>
+      </c>
+      <c r="Y4" s="16">
+        <v>-5</v>
+      </c>
+      <c r="Z4" s="16" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="5" spans="1:26">
       <c r="A5" s="11" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="C5" s="13">
         <v>44378</v>
@@ -956,16 +1036,16 @@
         <v>44384</v>
       </c>
       <c r="E5" s="14" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="F5" s="14">
-        <v>5668818</v>
+        <v>5671039</v>
       </c>
       <c r="G5" s="14" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="H5" s="14" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="I5" s="14" t="s">
         <v>25</v>
@@ -974,7 +1054,7 @@
         <v>25</v>
       </c>
       <c r="K5" s="14">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="L5" s="14">
         <v>30</v>
@@ -982,11 +1062,11 @@
       <c r="M5" s="14">
         <v>15</v>
       </c>
-      <c r="N5" s="14" t="s">
-        <v>50</v>
+      <c r="N5" s="15" t="s">
+        <v>41</v>
       </c>
       <c r="O5" s="16">
-        <v>100</v>
+        <v>85</v>
       </c>
       <c r="P5" s="11" t="s">
         <v>20</v>
@@ -995,13 +1075,13 @@
         <v>21</v>
       </c>
       <c r="R5" s="16" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="S5" s="16">
         <v>25</v>
       </c>
       <c r="T5" s="16">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="U5" s="16">
         <v>30</v>
@@ -1010,100 +1090,20 @@
         <v>15</v>
       </c>
       <c r="W5" s="17" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="X5" s="1">
-        <v>95</v>
+        <v>100</v>
       </c>
       <c r="Y5" s="16">
-        <v>-5</v>
-      </c>
-      <c r="Z5" s="16" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="6" spans="1:26">
-      <c r="A6" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="B6" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="C6" s="13">
-        <v>44378</v>
-      </c>
-      <c r="D6" s="13">
-        <v>44384</v>
-      </c>
-      <c r="E6" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="F6" s="14">
-        <v>5671039</v>
-      </c>
-      <c r="G6" s="14" t="s">
-        <v>43</v>
-      </c>
-      <c r="H6" s="14" t="s">
-        <v>42</v>
-      </c>
-      <c r="I6" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="J6" s="14">
-        <v>25</v>
-      </c>
-      <c r="K6" s="14">
         <v>15</v>
       </c>
-      <c r="L6" s="14">
-        <v>30</v>
-      </c>
-      <c r="M6" s="14">
-        <v>15</v>
-      </c>
-      <c r="N6" s="15" t="s">
-        <v>41</v>
-      </c>
-      <c r="O6" s="16">
-        <v>85</v>
-      </c>
-      <c r="P6" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q6" s="25" t="s">
-        <v>21</v>
-      </c>
-      <c r="R6" s="16" t="s">
-        <v>49</v>
-      </c>
-      <c r="S6" s="16">
-        <v>25</v>
-      </c>
-      <c r="T6" s="16">
-        <v>30</v>
-      </c>
-      <c r="U6" s="16">
-        <v>30</v>
-      </c>
-      <c r="V6" s="16">
-        <v>15</v>
-      </c>
-      <c r="W6" s="17" t="s">
-        <v>27</v>
-      </c>
-      <c r="X6" s="1">
-        <v>100</v>
-      </c>
-      <c r="Y6" s="16">
-        <v>15</v>
-      </c>
-      <c r="Z6" s="23" t="s">
+      <c r="Z5" s="23" t="s">
         <v>45</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A2:Z6"/>
+  <autoFilter ref="A1:Z5"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>